<commit_message>
Interim update to links files
</commit_message>
<xml_diff>
--- a/All_Links.xlsx
+++ b/All_Links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohnD'Amore\Source\Repos\ccda-search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A867C697-6E31-4593-ADDE-9830875D70F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF462C2A-9A20-4F1E-B816-877C36CF6000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1619" uniqueCount="1283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="1287">
   <si>
     <t>href="2.16.840.1.113883.10.20.22.1.4.html"&gt;Consultation</t>
   </si>
@@ -3888,6 +3888,18 @@
   </si>
   <si>
     <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1247.9/expansion/Latest</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/3.1.0/ValueSet-v3-HumanLanguage.html</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/2.0.0/CodeSystem-v3-nciThesaurus.html</t>
+  </si>
+  <si>
+    <t>Root for device IDs</t>
   </si>
 </sst>
 </file>
@@ -4324,21 +4336,27 @@
       <c r="C8">
         <v>0</v>
       </c>
+      <c r="D8" t="s">
+        <v>1283</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>904</v>
+        <v>606</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
         <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1285</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>724</v>
+        <v>769</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4349,7 +4367,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>606</v>
+        <v>63</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -4360,7 +4378,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>921</v>
+        <v>64</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4371,7 +4389,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>922</v>
+        <v>222</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4382,7 +4400,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>769</v>
+        <v>62</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4393,7 +4411,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>1127</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4404,7 +4422,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -4415,7 +4433,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>222</v>
+        <v>10</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -4426,7 +4444,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>149</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -4437,7 +4455,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>1127</v>
+        <v>167</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -4448,7 +4466,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>665</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -4459,7 +4477,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -4470,7 +4488,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>149</v>
+        <v>799</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -4481,7 +4499,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>167</v>
+        <v>667</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -4492,7 +4510,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>665</v>
+        <v>9</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -4503,7 +4521,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>200</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -4514,7 +4532,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>799</v>
+        <v>69</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -4525,7 +4543,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>667</v>
+        <v>124</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -4536,29 +4554,35 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>253</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
       <c r="C28">
         <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1273</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>200</v>
+        <v>1128</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29">
         <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1276</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>1254</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -4569,18 +4593,21 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>124</v>
+        <v>1129</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31">
         <v>0</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1274</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>253</v>
+        <v>1130</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -4589,26 +4616,23 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>1273</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1128</v>
+        <v>1131</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33">
         <v>0</v>
-      </c>
-      <c r="D33" t="s">
-        <v>1276</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>1254</v>
+        <v>725</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -4619,7 +4643,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1129</v>
+        <v>1132</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -4628,12 +4652,12 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>1130</v>
+        <v>694</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -4642,23 +4666,26 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>1131</v>
+        <v>422</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37">
         <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1270</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>725</v>
+        <v>502</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -4666,24 +4693,13 @@
       <c r="C38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>1132</v>
-      </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39" t="s">
-        <v>1272</v>
+      <c r="D38" t="s">
+        <v>1269</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>694</v>
+        <v>904</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -4692,12 +4708,12 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>1271</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>422</v>
+        <v>724</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -4706,12 +4722,12 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>1270</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>502</v>
+        <v>921</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -4720,7 +4736,18 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>1269</v>
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>922</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Commiting the link update excel and script
</commit_message>
<xml_diff>
--- a/All_Links.xlsx
+++ b/All_Links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohnD'Amore\Source\Repos\ccda-search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF462C2A-9A20-4F1E-B816-877C36CF6000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0303D8-9C1C-4330-936B-355D858E94AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="1287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="1312">
   <si>
     <t>href="2.16.840.1.113883.10.20.22.1.4.html"&gt;Consultation</t>
   </si>
@@ -3900,6 +3900,81 @@
   </si>
   <si>
     <t>Root for device IDs</t>
+  </si>
+  <si>
+    <t>n/a - health insurance</t>
+  </si>
+  <si>
+    <t>n/a US state</t>
+  </si>
+  <si>
+    <t>n/a US postla code</t>
+  </si>
+  <si>
+    <t>n/a coutnry code</t>
+  </si>
+  <si>
+    <t>n/a NUBC UB-04 FL17 Patient Status</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/3.1.0/CodeSystem-provenance-participant-type.html</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActMood.html</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActRelationshipType.html</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/1.0.0/CodeSystem-v3-NullFlavor.html</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/1.0.0/CodeSystem-v3-RoleClass.html</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/1.0.0/CodeSystem-v3-RoleCode.html</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActStatus.html</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActCode.html</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/1.0.0/CodeSystem-v3-EntityClass.html</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActClass.html</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/1.0.0/CodeSystem-v3-ParticipationFunction.html</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/1.0.0/CodeSystem-v3-ParticipationSignature.html</t>
+  </si>
+  <si>
+    <t>https://terminology.hl7.org/1.0.0/CodeSystem-v3-ParticipationType.html</t>
+  </si>
+  <si>
+    <t>n/a ICD-9</t>
+  </si>
+  <si>
+    <t>n/a ICF Self Care</t>
+  </si>
+  <si>
+    <t>NUBC UB-04 Patient Discharge Status code set</t>
+  </si>
+  <si>
+    <t>&lt;b&gt; &lt;a href="</t>
+  </si>
+  <si>
+    <t xml:space="preserve">" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; </t>
+  </si>
+  <si>
+    <t>&lt;/a&gt;&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>https://vsac.nlm.nih.gov/valueset/2.16.840.1.113883.1.11.12839/expansion/Latest</t>
   </si>
 </sst>
 </file>
@@ -4217,10 +4292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D396"/>
+  <dimension ref="A1:I397"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4228,10 +4303,10 @@
     <col min="1" max="1" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1257</v>
       </c>
@@ -4242,7 +4317,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>865</v>
       </c>
@@ -4255,8 +4330,25 @@
       <c r="D2" t="s">
         <v>1277</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H2" t="str">
+        <f>+E2&amp;D2&amp;F2&amp;A2&amp;G2</f>
+        <v>&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1021.101/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113762.1.4.1021.101&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I2" t="str">
+        <f>"'"&amp;A2&amp;"':"&amp;"'"&amp;H2&amp;"',"</f>
+        <v>'2.16.840.1.113762.1.4.1021.101':'&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1021.101/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113762.1.4.1021.101&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>747</v>
       </c>
@@ -4269,8 +4361,25 @@
       <c r="D3" t="s">
         <v>1278</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H29" si="0">+E3&amp;D3&amp;F3&amp;A3&amp;G3</f>
+        <v>&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1021.103/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113762.1.4.1021.103&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I30" si="1">"'"&amp;A3&amp;"':"&amp;"'"&amp;H3&amp;"',"</f>
+        <v>'2.16.840.1.113762.1.4.1021.103':'&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1021.103/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113762.1.4.1021.103&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>746</v>
       </c>
@@ -4283,8 +4392,25 @@
       <c r="D4" t="s">
         <v>1279</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1021.33/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113762.1.4.1021.33&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113762.1.4.1021.33':'&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1021.33/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113762.1.4.1021.33&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>866</v>
       </c>
@@ -4297,8 +4423,25 @@
       <c r="D5" t="s">
         <v>1280</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1114.17/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113762.1.4.1114.17&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113762.1.4.1114.17':'&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1114.17/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113762.1.4.1114.17&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>681</v>
       </c>
@@ -4311,8 +4454,25 @@
       <c r="D6" t="s">
         <v>1281</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1196.788/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113762.1.4.1196.788&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113762.1.4.1196.788':'&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1196.788/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113762.1.4.1196.788&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>924</v>
       </c>
@@ -4325,8 +4485,25 @@
       <c r="D7" t="s">
         <v>1282</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1247.9/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113762.1.4.1247.9&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113762.1.4.1247.9':'&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113762.1.4.1247.9/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113762.1.4.1247.9&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -4339,8 +4516,25 @@
       <c r="D8" t="s">
         <v>1283</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/3.1.0/ValueSet-v3-HumanLanguage.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.1.11.11526&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.1.11.11526':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/3.1.0/ValueSet-v3-HumanLanguage.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.1.11.11526&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>606</v>
       </c>
@@ -4353,262 +4547,679 @@
       <c r="D9" t="s">
         <v>1285</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/2.0.0/CodeSystem-v3-nciThesaurus.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.3.26.1.1&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.3.26.1.1':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/2.0.0/CodeSystem-v3-nciThesaurus.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.3.26.1.1&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1292</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/3.1.0/CodeSystem-provenance-participant-type.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.4.642.4.1131&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.4.642.4.1131':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/3.1.0/CodeSystem-provenance-participant-type.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.4.642.4.1131&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActMood.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.1001&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.5.1001':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActMood.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.1001&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1294</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActRelationshipType.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.1002&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.5.1002':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActRelationshipType.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.1002&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1295</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-NullFlavor.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.1008&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.5.1008':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-NullFlavor.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.1008&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1296</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-RoleClass.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.110&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.5.110':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-RoleClass.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.110&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>665</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1297</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-RoleCode.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.111&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.5.111':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-RoleCode.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.111&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1298</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActStatus.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.14&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.5.14':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActStatus.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.14&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>799</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1299</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H17" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActCode.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.4&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.5.4':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActCode.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.4&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>667</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1300</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-EntityClass.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.41&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.5.41':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-EntityClass.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.41&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1301</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActClass.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.6&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.5.6':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ActClass.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.6&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1302</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ParticipationFunction.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.88&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.5.88':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ParticipationFunction.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.88&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1303</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ParticipationSignature.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.89&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.5.89':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ParticipationSignature.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.89&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ParticipationType.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.90&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.5.90':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/1.0.0/CodeSystem-v3-ParticipationType.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.5.90&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>253</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1273</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-v3-loinc.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.1&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.6.1':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-v3-loinc.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.1&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-v3-nuccProviderCodes.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.101&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I24" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.6.101':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-v3-nuccProviderCodes.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.101&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1274</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-CPT.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.12&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.6.12':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-CPT.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.12&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-CDT.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.13&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.6.13':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-CDT.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.13&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1272</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-icd10PCS.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.4&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.6.4':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-icd10PCS.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.4&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>694</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-icd10CM.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.90&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.6.90':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-icd10CM.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.90&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>422</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1270</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-v3-snomed-CT.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.96&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.6.96':'&lt;b&gt; &lt;a href="https://terminology.hl7.org/CodeSystem-v3-snomed-CT.html" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.6.96&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>553</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1311</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1309</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" ref="H30" si="2">+E30&amp;D30&amp;F30&amp;A30&amp;G30</f>
+        <v>&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113883.1.11.12839/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.1.11.12839&lt;/a&gt;&lt;/b&gt;</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="1"/>
+        <v>'2.16.840.1.113883.1.11.12839':'&lt;b&gt; &lt;a href="https://vsac.nlm.nih.gov/valueset/2.16.840.1.113883.1.11.12839/expansion/Latest" target="_blank"&gt;&lt;i class="fas fa-external-link-alt"&gt;&lt;/i&gt; 2.16.840.1.113883.1.11.12839&lt;/a&gt;&lt;/b&gt;',</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>769</v>
       </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>222</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>1127</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>149</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>167</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>665</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>799</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>667</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>200</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>124</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>253</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28" t="s">
-        <v>1273</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>1128</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1276</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>1254</v>
-      </c>
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>1129</v>
-      </c>
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-      <c r="D31" t="s">
-        <v>1274</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>1130</v>
-      </c>
       <c r="B32">
         <v>0</v>
       </c>
@@ -4616,34 +5227,40 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>1275</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>1131</v>
+        <v>63</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33">
         <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1288</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>725</v>
+        <v>64</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34">
         <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1289</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>1132</v>
+        <v>222</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -4652,12 +5269,12 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>1272</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>694</v>
+        <v>62</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -4666,12 +5283,12 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>1271</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>422</v>
+        <v>1254</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -4680,12 +5297,12 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>1270</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>502</v>
+        <v>1131</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -4694,12 +5311,26 @@
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>1269</v>
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>725</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1307</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>904</v>
+        <v>502</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -4708,12 +5339,12 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>1284</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>724</v>
+        <v>904</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -4727,7 +5358,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>921</v>
+        <v>724</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -4736,23 +5367,26 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C43">
         <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1286</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>1111</v>
+        <v>922</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -4763,7 +5397,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -4774,7 +5408,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>1121</v>
+        <v>1112</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -4785,7 +5419,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>1237</v>
+        <v>1121</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -4796,7 +5430,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -4807,7 +5441,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>1255</v>
+        <v>1239</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -4818,7 +5452,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>916</v>
+        <v>1255</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -4829,7 +5463,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>1268</v>
+        <v>916</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -4840,7 +5474,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>917</v>
+        <v>1268</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -4851,7 +5485,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>1231</v>
+        <v>917</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -4862,7 +5496,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>1106</v>
+        <v>1231</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -4873,7 +5507,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -4884,7 +5518,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>919</v>
+        <v>1105</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -4895,7 +5529,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>1103</v>
+        <v>919</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -4906,7 +5540,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -4917,18 +5551,18 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>574</v>
+        <v>1104</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>1133</v>
+        <v>574</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -4939,7 +5573,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -4950,7 +5584,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -4961,7 +5595,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -4972,7 +5606,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -4983,7 +5617,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -4994,7 +5628,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -5005,7 +5639,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -5016,7 +5650,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -5027,7 +5661,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -5038,7 +5672,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -5049,7 +5683,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -5060,7 +5694,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -5071,7 +5705,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>693</v>
+        <v>1145</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -5082,7 +5716,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>1146</v>
+        <v>693</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -5093,7 +5727,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>212</v>
+        <v>1146</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -5104,7 +5738,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>1147</v>
+        <v>212</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -5115,7 +5749,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -5126,7 +5760,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -5137,7 +5771,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -5148,7 +5782,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -5159,7 +5793,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -5170,7 +5804,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -5181,7 +5815,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>553</v>
+        <v>1153</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -5192,7 +5826,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>1154</v>
+        <v>553</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -5203,7 +5837,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -5214,7 +5848,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -5225,7 +5859,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -5236,7 +5870,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -5247,7 +5881,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -5258,7 +5892,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -5269,7 +5903,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -5280,7 +5914,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -5291,7 +5925,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -5302,7 +5936,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -5313,7 +5947,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>1171</v>
+        <v>1164</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -5324,7 +5958,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>1165</v>
+        <v>1171</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -5335,7 +5969,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -5346,7 +5980,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -5357,7 +5991,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -5368,7 +6002,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -5379,7 +6013,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -5390,7 +6024,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -5401,7 +6035,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -5412,7 +6046,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -5423,7 +6057,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -5434,7 +6068,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -5445,7 +6079,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>851</v>
+        <v>1176</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -5456,7 +6090,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>1177</v>
+        <v>851</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -5467,7 +6101,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -5478,7 +6112,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>93</v>
+        <v>1178</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -5489,7 +6123,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>1179</v>
+        <v>93</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -5500,7 +6134,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -5511,7 +6145,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -5522,7 +6156,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>61</v>
+        <v>1181</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -5533,7 +6167,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>1182</v>
+        <v>61</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -5544,7 +6178,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -5555,7 +6189,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -5566,7 +6200,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -5577,7 +6211,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -5588,7 +6222,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>837</v>
+        <v>1186</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -5599,7 +6233,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>1126</v>
+        <v>837</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -5610,7 +6244,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>1187</v>
+        <v>1126</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -5621,7 +6255,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>71</v>
+        <v>1187</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -5632,7 +6266,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>1188</v>
+        <v>71</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -5643,7 +6277,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -5654,7 +6288,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -5665,7 +6299,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -5676,7 +6310,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>815</v>
+        <v>1191</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -5687,7 +6321,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>1192</v>
+        <v>815</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -5698,7 +6332,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -5709,7 +6343,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -5720,7 +6354,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -5731,7 +6365,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -5742,7 +6376,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -5753,7 +6387,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -5764,7 +6398,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -5775,7 +6409,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>920</v>
+        <v>1199</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -5786,7 +6420,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>1200</v>
+        <v>920</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -5797,7 +6431,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -5808,7 +6442,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -5819,7 +6453,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -5830,7 +6464,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -5841,7 +6475,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -5852,7 +6486,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -5863,7 +6497,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -5874,7 +6508,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -5885,7 +6519,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -5896,7 +6530,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -5907,7 +6541,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -5918,7 +6552,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -5929,7 +6563,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>691</v>
+        <v>1212</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -5940,7 +6574,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>1213</v>
+        <v>691</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -5951,7 +6585,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -5962,7 +6596,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -5973,7 +6607,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>202</v>
+        <v>1215</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -5984,7 +6618,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>923</v>
+        <v>202</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -5995,7 +6629,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>1216</v>
+        <v>923</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -6006,7 +6640,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -6017,7 +6651,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -6028,7 +6662,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -6039,7 +6673,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -6050,7 +6684,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>68</v>
+        <v>1220</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -6061,7 +6695,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>1221</v>
+        <v>68</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -6072,7 +6706,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -6083,26 +6717,29 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B165">
+        <v>0</v>
+      </c>
+      <c r="C165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
         <v>1223</v>
       </c>
-      <c r="B165">
-        <v>0</v>
-      </c>
-      <c r="C165">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
-        <v>1074</v>
-      </c>
-      <c r="B167">
+      <c r="B166">
+        <v>0</v>
+      </c>
+      <c r="C166">
         <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>1001</v>
+        <v>1074</v>
       </c>
       <c r="B168">
         <v>1</v>
@@ -6110,7 +6747,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>925</v>
+        <v>1001</v>
       </c>
       <c r="B169">
         <v>1</v>
@@ -6118,7 +6755,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B170">
         <v>1</v>
@@ -6126,7 +6763,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B171">
         <v>1</v>
@@ -6134,7 +6771,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B172">
         <v>1</v>
@@ -6142,7 +6779,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B173">
         <v>1</v>
@@ -6150,7 +6787,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B174">
         <v>1</v>
@@ -6158,7 +6795,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B175">
         <v>1</v>
@@ -6166,7 +6803,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B176">
         <v>1</v>
@@ -6174,7 +6811,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B177">
         <v>1</v>
@@ -6182,7 +6819,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B178">
         <v>1</v>
@@ -6190,7 +6827,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>1224</v>
+        <v>934</v>
       </c>
       <c r="B179">
         <v>1</v>
@@ -6198,7 +6835,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="B180">
         <v>1</v>
@@ -6206,7 +6843,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="B181">
         <v>1</v>
@@ -6214,7 +6851,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B182">
         <v>1</v>
@@ -6222,7 +6859,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="B183">
         <v>1</v>
@@ -6230,7 +6867,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="B184">
         <v>1</v>
@@ -6238,7 +6875,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="B185">
         <v>1</v>
@@ -6246,7 +6883,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="B186">
         <v>1</v>
@@ -6254,7 +6891,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="B187">
         <v>1</v>
@@ -6262,7 +6899,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="B188">
         <v>1</v>
@@ -6270,7 +6907,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="B189">
         <v>1</v>
@@ -6278,7 +6915,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B190">
         <v>1</v>
@@ -6286,7 +6923,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="B191">
         <v>1</v>
@@ -6294,7 +6931,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>935</v>
+        <v>1238</v>
       </c>
       <c r="B192">
         <v>1</v>
@@ -6302,7 +6939,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B193">
         <v>1</v>
@@ -6310,7 +6947,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>912</v>
+        <v>936</v>
       </c>
       <c r="B194">
         <v>1</v>
@@ -6318,7 +6955,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>937</v>
+        <v>912</v>
       </c>
       <c r="B195">
         <v>1</v>
@@ -6326,7 +6963,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B196">
         <v>1</v>
@@ -6334,7 +6971,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>913</v>
+        <v>938</v>
       </c>
       <c r="B197">
         <v>1</v>
@@ -6342,7 +6979,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B198">
         <v>1</v>
@@ -6350,7 +6987,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>939</v>
+        <v>914</v>
       </c>
       <c r="B199">
         <v>1</v>
@@ -6358,7 +6995,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B200">
         <v>1</v>
@@ -6366,7 +7003,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B201">
         <v>1</v>
@@ -6374,7 +7011,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B202">
         <v>1</v>
@@ -6382,7 +7019,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B203">
         <v>1</v>
@@ -6390,7 +7027,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B204">
         <v>1</v>
@@ -6398,7 +7035,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B205">
         <v>1</v>
@@ -6406,7 +7043,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B206">
         <v>1</v>
@@ -6414,7 +7051,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B207">
         <v>1</v>
@@ -6422,7 +7059,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B208">
         <v>1</v>
@@ -6430,7 +7067,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B209">
         <v>1</v>
@@ -6438,7 +7075,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B210">
         <v>1</v>
@@ -6446,7 +7083,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B211">
         <v>1</v>
@@ -6454,7 +7091,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B212">
         <v>1</v>
@@ -6462,7 +7099,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B213">
         <v>1</v>
@@ -6470,7 +7107,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>1240</v>
+        <v>953</v>
       </c>
       <c r="B214">
         <v>1</v>
@@ -6478,7 +7115,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>954</v>
+        <v>1240</v>
       </c>
       <c r="B215">
         <v>1</v>
@@ -6486,7 +7123,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B216">
         <v>1</v>
@@ -6494,7 +7131,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B217">
         <v>1</v>
@@ -6502,7 +7139,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B218">
         <v>1</v>
@@ -6510,7 +7147,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B219">
         <v>1</v>
@@ -6518,7 +7155,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B220">
         <v>1</v>
@@ -6526,7 +7163,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B221">
         <v>1</v>
@@ -6534,7 +7171,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>1241</v>
+        <v>960</v>
       </c>
       <c r="B222">
         <v>1</v>
@@ -6542,7 +7179,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>961</v>
+        <v>1241</v>
       </c>
       <c r="B223">
         <v>1</v>
@@ -6550,7 +7187,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B224">
         <v>1</v>
@@ -6558,7 +7195,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B225">
         <v>1</v>
@@ -6566,7 +7203,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B226">
         <v>1</v>
@@ -6574,7 +7211,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B227">
         <v>1</v>
@@ -6582,7 +7219,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B228">
         <v>1</v>
@@ -6590,7 +7227,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B229">
         <v>1</v>
@@ -6598,7 +7235,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B230">
         <v>1</v>
@@ -6606,7 +7243,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B231">
         <v>1</v>
@@ -6614,7 +7251,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B232">
         <v>1</v>
@@ -6622,7 +7259,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B233">
         <v>1</v>
@@ -6630,7 +7267,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B234">
         <v>1</v>
@@ -6638,7 +7275,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B235">
         <v>1</v>
@@ -6646,7 +7283,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B236">
         <v>1</v>
@@ -6654,7 +7291,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B237">
         <v>1</v>
@@ -6662,7 +7299,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B238">
         <v>1</v>
@@ -6670,7 +7307,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>1242</v>
+        <v>976</v>
       </c>
       <c r="B239">
         <v>1</v>
@@ -6678,7 +7315,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>977</v>
+        <v>1242</v>
       </c>
       <c r="B240">
         <v>1</v>
@@ -6686,7 +7323,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B241">
         <v>1</v>
@@ -6694,7 +7331,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B242">
         <v>1</v>
@@ -6702,7 +7339,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B243">
         <v>1</v>
@@ -6710,7 +7347,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B244">
         <v>1</v>
@@ -6718,7 +7355,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B245">
         <v>1</v>
@@ -6726,7 +7363,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B246">
         <v>1</v>
@@ -6734,7 +7371,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="B247">
         <v>1</v>
@@ -6742,7 +7379,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>1243</v>
+        <v>984</v>
       </c>
       <c r="B248">
         <v>1</v>
@@ -6750,7 +7387,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>985</v>
+        <v>1243</v>
       </c>
       <c r="B249">
         <v>1</v>
@@ -6758,7 +7395,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B250">
         <v>1</v>
@@ -6766,7 +7403,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>406</v>
+        <v>986</v>
       </c>
       <c r="B251">
         <v>1</v>
@@ -6774,7 +7411,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>915</v>
+        <v>406</v>
       </c>
       <c r="B252">
         <v>1</v>
@@ -6782,7 +7419,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>987</v>
+        <v>915</v>
       </c>
       <c r="B253">
         <v>1</v>
@@ -6790,7 +7427,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B254">
         <v>1</v>
@@ -6798,7 +7435,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="B255">
         <v>1</v>
@@ -6806,7 +7443,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="B256">
         <v>1</v>
@@ -6814,7 +7451,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="B257">
         <v>1</v>
@@ -6822,7 +7459,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B258">
         <v>1</v>
@@ -6830,7 +7467,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B259">
         <v>1</v>
@@ -6838,7 +7475,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B260">
         <v>1</v>
@@ -6846,7 +7483,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B261">
         <v>1</v>
@@ -6854,7 +7491,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B262">
         <v>1</v>
@@ -6862,7 +7499,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B263">
         <v>1</v>
@@ -6870,7 +7507,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B264">
         <v>1</v>
@@ -6878,7 +7515,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B265">
         <v>1</v>
@@ -6886,7 +7523,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B266">
         <v>1</v>
@@ -6894,7 +7531,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B267">
         <v>1</v>
@@ -6902,7 +7539,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B268">
         <v>1</v>
@@ -6910,7 +7547,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B269">
         <v>1</v>
@@ -6918,7 +7555,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B270">
         <v>1</v>
@@ -6926,7 +7563,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B271">
         <v>1</v>
@@ -6934,7 +7571,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B272">
         <v>1</v>
@@ -6942,7 +7579,7 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B273">
         <v>1</v>
@@ -6950,7 +7587,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B274">
         <v>1</v>
@@ -6958,7 +7595,7 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B275">
         <v>1</v>
@@ -6966,7 +7603,7 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B276">
         <v>1</v>
@@ -6974,7 +7611,7 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B277">
         <v>1</v>
@@ -6982,7 +7619,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B278">
         <v>1</v>
@@ -6990,7 +7627,7 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B279">
         <v>1</v>
@@ -6998,7 +7635,7 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B280">
         <v>1</v>
@@ -7006,7 +7643,7 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B281">
         <v>1</v>
@@ -7014,7 +7651,7 @@
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B282">
         <v>1</v>
@@ -7022,7 +7659,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B283">
         <v>1</v>
@@ -7030,7 +7667,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B284">
         <v>1</v>
@@ -7038,7 +7675,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B285">
         <v>1</v>
@@ -7046,7 +7683,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B286">
         <v>1</v>
@@ -7054,7 +7691,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B287">
         <v>1</v>
@@ -7062,7 +7699,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B288">
         <v>1</v>
@@ -7070,7 +7707,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B289">
         <v>1</v>
@@ -7078,7 +7715,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B290">
         <v>1</v>
@@ -7086,7 +7723,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B291">
         <v>1</v>
@@ -7094,7 +7731,7 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B292">
         <v>1</v>
@@ -7102,7 +7739,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B293">
         <v>1</v>
@@ -7110,7 +7747,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B294">
         <v>1</v>
@@ -7118,7 +7755,7 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>1244</v>
+        <v>1028</v>
       </c>
       <c r="B295">
         <v>1</v>
@@ -7126,7 +7763,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="B296">
         <v>1</v>
@@ -7134,7 +7771,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>1029</v>
+        <v>1245</v>
       </c>
       <c r="B297">
         <v>1</v>
@@ -7142,7 +7779,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="B298">
         <v>1</v>
@@ -7150,7 +7787,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B299">
         <v>1</v>
@@ -7158,7 +7795,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B300">
         <v>1</v>
@@ -7166,7 +7803,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="B301">
         <v>1</v>
@@ -7174,7 +7811,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B302">
         <v>1</v>
@@ -7182,7 +7819,7 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B303">
         <v>1</v>
@@ -7190,7 +7827,7 @@
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B304">
         <v>1</v>
@@ -7198,7 +7835,7 @@
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B305">
         <v>1</v>
@@ -7206,7 +7843,7 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B306">
         <v>1</v>
@@ -7214,7 +7851,7 @@
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B307">
         <v>1</v>
@@ -7222,7 +7859,7 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B308">
         <v>1</v>
@@ -7230,7 +7867,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B309">
         <v>1</v>
@@ -7238,7 +7875,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B310">
         <v>1</v>
@@ -7246,7 +7883,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B311">
         <v>1</v>
@@ -7254,7 +7891,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="B312">
         <v>1</v>
@@ -7262,7 +7899,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B313">
         <v>1</v>
@@ -7270,7 +7907,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>1246</v>
+        <v>1045</v>
       </c>
       <c r="B314">
         <v>1</v>
@@ -7278,7 +7915,7 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>1046</v>
+        <v>1246</v>
       </c>
       <c r="B315">
         <v>1</v>
@@ -7286,7 +7923,7 @@
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B316">
         <v>1</v>
@@ -7294,7 +7931,7 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B317">
         <v>1</v>
@@ -7302,7 +7939,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B318">
         <v>1</v>
@@ -7310,7 +7947,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B319">
         <v>1</v>
@@ -7318,7 +7955,7 @@
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B320">
         <v>1</v>
@@ -7326,7 +7963,7 @@
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="B321">
         <v>1</v>
@@ -7334,7 +7971,7 @@
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B322">
         <v>1</v>
@@ -7342,7 +7979,7 @@
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B323">
         <v>1</v>
@@ -7350,7 +7987,7 @@
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="B324">
         <v>1</v>
@@ -7358,7 +7995,7 @@
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="B325">
         <v>1</v>
@@ -7366,7 +8003,7 @@
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>604</v>
+        <v>1056</v>
       </c>
       <c r="B326">
         <v>1</v>
@@ -7374,7 +8011,7 @@
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>1057</v>
+        <v>604</v>
       </c>
       <c r="B327">
         <v>1</v>
@@ -7382,7 +8019,7 @@
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B328">
         <v>1</v>
@@ -7390,7 +8027,7 @@
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B329">
         <v>1</v>
@@ -7398,7 +8035,7 @@
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B330">
         <v>1</v>
@@ -7406,7 +8043,7 @@
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B331">
         <v>1</v>
@@ -7414,7 +8051,7 @@
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B332">
         <v>1</v>
@@ -7422,7 +8059,7 @@
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="B333">
         <v>1</v>
@@ -7430,7 +8067,7 @@
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B334">
         <v>1</v>
@@ -7438,7 +8075,7 @@
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B335">
         <v>1</v>
@@ -7446,7 +8083,7 @@
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="B336">
         <v>1</v>
@@ -7454,7 +8091,7 @@
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B337">
         <v>1</v>
@@ -7462,7 +8099,7 @@
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B338">
         <v>1</v>
@@ -7470,7 +8107,7 @@
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B339">
         <v>1</v>
@@ -7478,7 +8115,7 @@
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B340">
         <v>1</v>
@@ -7486,7 +8123,7 @@
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B341">
         <v>1</v>
@@ -7494,7 +8131,7 @@
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B342">
         <v>1</v>
@@ -7502,7 +8139,7 @@
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="B343">
         <v>1</v>
@@ -7510,7 +8147,7 @@
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="B344">
         <v>1</v>
@@ -7518,7 +8155,7 @@
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>1247</v>
+        <v>1075</v>
       </c>
       <c r="B345">
         <v>1</v>
@@ -7526,7 +8163,7 @@
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
-        <v>1076</v>
+        <v>1247</v>
       </c>
       <c r="B346">
         <v>1</v>
@@ -7534,7 +8171,7 @@
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B347">
         <v>1</v>
@@ -7542,7 +8179,7 @@
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B348">
         <v>1</v>
@@ -7550,7 +8187,7 @@
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B349">
         <v>1</v>
@@ -7558,7 +8195,7 @@
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B350">
         <v>1</v>
@@ -7566,7 +8203,7 @@
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B351">
         <v>1</v>
@@ -7574,7 +8211,7 @@
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B352">
         <v>1</v>
@@ -7582,7 +8219,7 @@
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B353">
         <v>1</v>
@@ -7590,7 +8227,7 @@
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B354">
         <v>1</v>
@@ -7598,7 +8235,7 @@
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>1248</v>
+        <v>1084</v>
       </c>
       <c r="B355">
         <v>1</v>
@@ -7606,7 +8243,7 @@
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
-        <v>1085</v>
+        <v>1248</v>
       </c>
       <c r="B356">
         <v>1</v>
@@ -7614,7 +8251,7 @@
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B357">
         <v>1</v>
@@ -7622,7 +8259,7 @@
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B358">
         <v>1</v>
@@ -7630,7 +8267,7 @@
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B359">
         <v>1</v>
@@ -7638,7 +8275,7 @@
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B360">
         <v>1</v>
@@ -7646,7 +8283,7 @@
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B361">
         <v>1</v>
@@ -7654,7 +8291,7 @@
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B362">
         <v>1</v>
@@ -7662,7 +8299,7 @@
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B363">
         <v>1</v>
@@ -7670,7 +8307,7 @@
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B364">
         <v>1</v>
@@ -7678,7 +8315,7 @@
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B365">
         <v>1</v>
@@ -7686,7 +8323,7 @@
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B366">
         <v>1</v>
@@ -7694,7 +8331,7 @@
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B367">
         <v>1</v>
@@ -7702,7 +8339,7 @@
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B368">
         <v>1</v>
@@ -7710,7 +8347,7 @@
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
-        <v>918</v>
+        <v>1097</v>
       </c>
       <c r="B369">
         <v>1</v>
@@ -7718,7 +8355,7 @@
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
-        <v>1249</v>
+        <v>918</v>
       </c>
       <c r="B370">
         <v>1</v>
@@ -7726,7 +8363,7 @@
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
-        <v>1098</v>
+        <v>1249</v>
       </c>
       <c r="B371">
         <v>1</v>
@@ -7734,7 +8371,7 @@
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B372">
         <v>1</v>
@@ -7742,7 +8379,7 @@
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B373">
         <v>1</v>
@@ -7750,7 +8387,7 @@
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B374">
         <v>1</v>
@@ -7758,7 +8395,7 @@
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B375">
         <v>1</v>
@@ -7766,7 +8403,7 @@
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
-        <v>1250</v>
+        <v>1102</v>
       </c>
       <c r="B376">
         <v>1</v>
@@ -7774,7 +8411,7 @@
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="B377">
         <v>1</v>
@@ -7782,7 +8419,7 @@
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>1107</v>
+        <v>1251</v>
       </c>
       <c r="B378">
         <v>1</v>
@@ -7790,7 +8427,7 @@
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
-        <v>1252</v>
+        <v>1107</v>
       </c>
       <c r="B379">
         <v>1</v>
@@ -7798,7 +8435,7 @@
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B380">
         <v>1</v>
@@ -7806,7 +8443,7 @@
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
-        <v>1108</v>
+        <v>1253</v>
       </c>
       <c r="B381">
         <v>1</v>
@@ -7814,7 +8451,7 @@
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B382">
         <v>1</v>
@@ -7822,7 +8459,7 @@
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B383">
         <v>1</v>
@@ -7830,7 +8467,7 @@
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="B384">
         <v>1</v>
@@ -7838,7 +8475,7 @@
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B385">
         <v>1</v>
@@ -7846,7 +8483,7 @@
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B386">
         <v>1</v>
@@ -7854,7 +8491,7 @@
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B387">
         <v>1</v>
@@ -7862,7 +8499,7 @@
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B388">
         <v>1</v>
@@ -7870,7 +8507,7 @@
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B389">
         <v>1</v>
@@ -7878,7 +8515,7 @@
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B390">
         <v>1</v>
@@ -7886,7 +8523,7 @@
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B391">
         <v>1</v>
@@ -7894,7 +8531,7 @@
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="B392">
         <v>1</v>
@@ -7902,7 +8539,7 @@
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B393">
         <v>1</v>
@@ -7910,7 +8547,7 @@
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B394">
         <v>1</v>
@@ -7918,7 +8555,7 @@
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B395">
         <v>1</v>
@@ -7926,15 +8563,23 @@
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B396">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A397" t="s">
         <v>1256</v>
       </c>
-      <c r="B396">
+      <c r="B397">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C165">
-    <sortCondition ref="C2:C165"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C166">
+    <sortCondition ref="C2:C166"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>